<commit_message>
note added, character "Indenfor"
</commit_message>
<xml_diff>
--- a/Rolleliste.xlsx
+++ b/Rolleliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ullakallenbach/Dropbox/FORSKNING/Kulturarvscluster/P017_R_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8418D0B9-7E92-3540-A6B4-67204DA16D1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1067A970-64F8-C84B-ABEA-CD63767FC320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7420" yWindow="500" windowWidth="21000" windowHeight="16940" xr2:uid="{CB4EA0A2-2CDD-6E44-9382-313F495EEF1B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="235">
   <si>
     <t>Barselskvinden</t>
   </si>
@@ -734,6 +734,12 @@
   </si>
   <si>
     <t>Pigen, En pige, 1. pige</t>
+  </si>
+  <si>
+    <t>Indenfor</t>
+  </si>
+  <si>
+    <t>der er en karakter, der hedder indenfor…</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E2D2AA-8F7A-E44B-B236-98A48F3AAF14}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2149,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3EF882-6F0E-6449-BF3F-52DA3CC48D65}">
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2349,6 +2355,17 @@
         <v>182</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Kørt nye grafer, rolleliste opdateret
</commit_message>
<xml_diff>
--- a/Rolleliste.xlsx
+++ b/Rolleliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ullakallenbach/Dropbox/FORSKNING/Kulturarvscluster/P017_R_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933AE31A-912D-AA41-92C0-FEC405AD21EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2D838E-7E93-E14E-8A42-882C7DB4F525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21000" windowHeight="16940" xr2:uid="{CB4EA0A2-2CDD-6E44-9382-313F495EEF1B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21000" windowHeight="16940" activeTab="1" xr2:uid="{CB4EA0A2-2CDD-6E44-9382-313F495EEF1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Karakterer og alias" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="254">
   <si>
     <t>Barselskvinden</t>
   </si>
@@ -391,12 +391,6 @@
     <t>manden i portechaisen</t>
   </si>
   <si>
-    <t>Drengen, En dreng, Dreng, En Dreng</t>
-  </si>
-  <si>
-    <t>Drengen [Jan]</t>
-  </si>
-  <si>
     <t>5 husfolk</t>
   </si>
   <si>
@@ -715,9 +709,6 @@
     <t>Indenfor</t>
   </si>
   <si>
-    <t>der er en karakter, der hedder indenfor…</t>
-  </si>
-  <si>
     <t>Barselskvinde, Barselskonen, Barselsquinde, Barselskvinden, Barselsqvinde</t>
   </si>
   <si>
@@ -800,6 +791,12 @@
   </si>
   <si>
     <t>Mandane, Mandane.</t>
+  </si>
+  <si>
+    <t>Drengen, En dreng, Dreng, En Dreng, Jan</t>
+  </si>
+  <si>
+    <t>det er studerende, der råber offstage</t>
   </si>
 </sst>
 </file>
@@ -1178,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E2D2AA-8F7A-E44B-B236-98A48F3AAF14}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView topLeftCell="A64" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1249,10 +1246,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1318,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1345,7 +1342,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
@@ -1356,7 +1353,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s">
         <v>67</v>
@@ -1367,7 +1364,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
@@ -1378,7 +1375,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1389,7 +1386,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B19" t="s">
         <v>72</v>
@@ -1400,7 +1397,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s">
         <v>74</v>
@@ -1411,7 +1408,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
@@ -1433,95 +1430,95 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B30" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
         <v>79</v>
@@ -1532,7 +1529,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B32" t="s">
         <v>76</v>
@@ -1543,7 +1540,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
@@ -1554,7 +1551,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B34" t="s">
         <v>84</v>
@@ -1565,7 +1562,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B35" t="s">
         <v>86</v>
@@ -1576,123 +1573,123 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" t="s">
         <v>139</v>
-      </c>
-      <c r="B37" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" t="s">
         <v>195</v>
-      </c>
-      <c r="B40" t="s">
-        <v>196</v>
-      </c>
-      <c r="C40" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C41" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C42" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B44" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C44" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B45" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C45" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1711,10 +1708,10 @@
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1766,103 +1763,103 @@
         <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
         <v>144</v>
       </c>
-      <c r="B55" t="s">
-        <v>146</v>
-      </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" t="s">
         <v>148</v>
-      </c>
-      <c r="C56" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B57" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B60" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C61" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B62" t="s">
         <v>63</v>
@@ -1939,123 +1936,123 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B69" t="s">
         <v>58</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C71" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
       </c>
       <c r="C72" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B73" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C73" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
         <v>40</v>
       </c>
       <c r="C74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C76" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C77" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C78" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B79" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2104,24 +2101,24 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B85" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C85" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2209,51 +2206,51 @@
         <v>52</v>
       </c>
       <c r="C93" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>239</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>245</v>
-      </c>
       <c r="C95" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B96" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C96" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B97" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C97" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2268,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3EF882-6F0E-6449-BF3F-52DA3CC48D65}">
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2284,13 +2281,13 @@
         <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
         <v>115</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2304,7 +2301,7 @@
         <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2318,7 +2315,7 @@
         <v>115</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2326,24 +2323,24 @@
         <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2351,7 +2348,7 @@
         <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2362,10 +2359,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2373,10 +2370,10 @@
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2387,7 +2384,7 @@
         <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2395,10 +2392,10 @@
         <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2406,147 +2403,147 @@
         <v>88</v>
       </c>
       <c r="B13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" t="s">
         <v>166</v>
-      </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" t="s">
         <v>169</v>
-      </c>
-      <c r="D15" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" t="s">
         <v>173</v>
-      </c>
-      <c r="D18" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C23" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D23" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
         <v>139</v>
       </c>
-      <c r="B27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" t="s">
-        <v>141</v>
-      </c>
       <c r="D27" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C30" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2554,10 +2551,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B35" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
opdateret grafer og rolleliste
</commit_message>
<xml_diff>
--- a/Rolleliste.xlsx
+++ b/Rolleliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ullakallenbach/Dropbox/FORSKNING/Kulturarvscluster/P017_R_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B6FBE0-0DE8-F44D-9E1D-607E392B52BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8C7CA-0819-834A-81A1-94DEEC25948D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="500" windowWidth="24020" windowHeight="16940" xr2:uid="{CB4EA0A2-2CDD-6E44-9382-313F495EEF1B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="265">
   <si>
     <t>Barselskvinden</t>
   </si>
@@ -166,9 +166,6 @@
     <t xml:space="preserve">Den usynliges broder </t>
   </si>
   <si>
-    <t xml:space="preserve">Den usynliges [Magdelones] broder </t>
-  </si>
-  <si>
     <t>Cosmoligoreus</t>
   </si>
   <si>
@@ -550,9 +547,6 @@
     <t>Der er både fremmede (2 personer der taler), den fremmede og en anden fremmed. Sidstenævnte fremgår ikke i rolleoversigten</t>
   </si>
   <si>
-    <t>Indenfor fremstår som en rolle</t>
-  </si>
-  <si>
     <t>Nytaarsprolog_mod.jsonl</t>
   </si>
   <si>
@@ -830,13 +824,19 @@
   </si>
   <si>
     <t>Tredje proprietær</t>
+  </si>
+  <si>
+    <t>Den usynlige</t>
+  </si>
+  <si>
+    <t>er både "Leonora", Columbine, og Magdelone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -865,6 +865,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -886,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -894,6 +900,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1210,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E2D2AA-8F7A-E44B-B236-98A48F3AAF14}">
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,57 +1252,57 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>245</v>
+        <v>234</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,10 +1321,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,10 +1332,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,10 +1343,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1347,10 +1354,10 @@
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1358,10 +1365,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1369,10 +1376,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1390,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1391,10 +1398,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1405,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1432,79 +1439,79 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1512,7 +1519,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>42</v>
@@ -1520,299 +1527,299 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B42" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1831,10 +1838,10 @@
         <v>14</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1842,10 +1849,10 @@
         <v>14</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -1886,109 +1893,109 @@
         <v>14</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1996,7 +2003,7 @@
         <v>34</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>35</v>
@@ -2018,7 +2025,7 @@
         <v>26</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>29</v>
@@ -2048,145 +2055,145 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="C88" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2202,156 +2209,156 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="C90" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B92" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C92" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B93" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B94" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C94" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="C97" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C98" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B99" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="C100" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B103" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="C103" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2375,287 +2382,290 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3EF882-6F0E-6449-BF3F-52DA3CC48D65}">
-  <dimension ref="A2:E34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" t="s">
+        <v>264</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
         <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="B6" t="s">
-        <v>125</v>
-      </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" t="s">
         <v>157</v>
-      </c>
-      <c r="D9" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" t="s">
         <v>162</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>163</v>
-      </c>
-      <c r="D13" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" t="s">
         <v>165</v>
       </c>
-      <c r="B14" t="s">
-        <v>166</v>
-      </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" t="s">
         <v>169</v>
-      </c>
-      <c r="D17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" t="s">
         <v>136</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>137</v>
       </c>
-      <c r="C27" t="s">
-        <v>138</v>
-      </c>
       <c r="D27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" t="s">
         <v>165</v>
-      </c>
-      <c r="C29" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" t="s">
+        <v>228</v>
+      </c>
+      <c r="D30" t="s">
         <v>229</v>
-      </c>
-      <c r="C30" t="s">
-        <v>230</v>
-      </c>
-      <c r="D30" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
@@ -2663,10 +2673,10 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>